<commit_message>
Adjust to model functions
</commit_message>
<xml_diff>
--- a/data/Benthic_1.xlsx
+++ b/data/Benthic_1.xlsx
@@ -493,6 +493,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -690,10 +691,10 @@
   <dimension ref="A1:G15"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="L2:L10 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.7421875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.75" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="11.42"/>
   </cols>
@@ -824,11 +825,11 @@
   </sheetPr>
   <dimension ref="A1:M1033"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="J1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L2" activeCellId="0" sqref="L2:L10"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D4" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="M32" activeCellId="0" sqref="M32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.7421875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.75" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="14.98"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="7" style="0" width="18.85"/>
@@ -999,7 +1000,7 @@
         <v>33</v>
       </c>
       <c r="M4" s="0" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1081,7 +1082,7 @@
         <v>35</v>
       </c>
       <c r="M6" s="0" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1327,7 +1328,7 @@
         <v>43</v>
       </c>
       <c r="M12" s="0" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1450,7 +1451,7 @@
         <v>46</v>
       </c>
       <c r="M15" s="0" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1655,7 +1656,7 @@
         <v>51</v>
       </c>
       <c r="M20" s="0" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1901,7 +1902,7 @@
         <v>40</v>
       </c>
       <c r="M26" s="0" t="n">
-        <v>64</v>
+        <v>60</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2106,7 +2107,7 @@
         <v>38</v>
       </c>
       <c r="M31" s="0" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2147,7 +2148,7 @@
         <v>40</v>
       </c>
       <c r="M32" s="0" t="n">
-        <v>40</v>
+        <v>35</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -6532,10 +6533,10 @@
   <dimension ref="A1:M513"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E7" activeCellId="1" sqref="L2:L10 E7"/>
+      <selection pane="topLeft" activeCell="M2" activeCellId="0" sqref="M2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.7421875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.75" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="7" style="0" width="12.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="14.69"/>
@@ -6625,7 +6626,7 @@
         <v>59</v>
       </c>
       <c r="M2" s="0" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7238,10 +7239,10 @@
   <dimension ref="A1:X119"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F76" activeCellId="1" sqref="L2:L10 F76"/>
+      <selection pane="topLeft" activeCell="G1" activeCellId="0" sqref="G1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.7421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.75" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="7" style="0" width="12.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="14.69"/>

</xml_diff>